<commit_message>
eddy ni 1992-1993 (update 2)
</commit_message>
<xml_diff>
--- a/_data/ni/ni9293/individueel_eindstand_dworp_123_9293.xlsx
+++ b/_data/ni/ni9293/individueel_eindstand_dworp_123_9293.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="-15" windowWidth="14310" windowHeight="12840" activeTab="12"/>
+    <workbookView xWindow="14505" yWindow="-15" windowWidth="14310" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -595,9 +595,6 @@
     <t>Carnières</t>
   </si>
   <si>
-    <t>Montigny</t>
-  </si>
-  <si>
     <t>4C</t>
   </si>
   <si>
@@ -614,6 +611,9 @@
   </si>
   <si>
     <t>Jumet 2</t>
+  </si>
+  <si>
+    <t>Montignies</t>
   </si>
 </sst>
 </file>
@@ -1734,9 +1734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1772,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1780,7 +1778,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1788,7 +1786,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1">
@@ -2066,7 +2064,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2116,7 +2114,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -2128,7 +2126,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -2138,7 +2136,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -2150,7 +2148,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -2160,7 +2158,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -2172,7 +2170,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -2182,7 +2180,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -2196,7 +2194,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -3774,7 +3772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AQ280"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5997,7 +5995,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C20" s="40">
         <v>1.5</v>
@@ -7020,7 +7018,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C27" s="69">
         <v>0</v>
@@ -18535,8 +18533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18791,7 +18789,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>

</xml_diff>